<commit_message>
penambahan bab 3 : flowchat,diagram flow dan use case
</commit_message>
<xml_diff>
--- a/01 LAPORAN/PRIRI_NORMALIASI_ERD.xlsx
+++ b/01 LAPORAN/PRIRI_NORMALIASI_ERD.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="31">
   <si>
     <t>UNF</t>
   </si>
@@ -240,7 +240,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -423,11 +423,111 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -455,12 +555,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -479,31 +581,6 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -522,7 +599,63 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -875,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AB91"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,87 +1036,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="31"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="37"/>
     </row>
     <row r="2" spans="3:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="32"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="33"/>
-      <c r="AA2" s="34"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="39"/>
+      <c r="X2" s="39"/>
+      <c r="Y2" s="39"/>
+      <c r="Z2" s="39"/>
+      <c r="AA2" s="40"/>
     </row>
     <row r="3" spans="3:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="32"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="33"/>
-      <c r="W3" s="33"/>
-      <c r="X3" s="33"/>
-      <c r="Y3" s="33"/>
-      <c r="Z3" s="33"/>
-      <c r="AA3" s="34"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="40"/>
     </row>
     <row r="4" spans="3:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="C4" s="11"/>
@@ -1013,12 +1146,12 @@
       <c r="AA4" s="13"/>
     </row>
     <row r="5" spans="3:28" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
@@ -1118,7 +1251,7 @@
       <c r="C8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="27" t="s">
         <v>27</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -1154,7 +1287,7 @@
       <c r="C9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="27" t="s">
         <v>28</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -1243,23 +1376,23 @@
       <c r="AB11" s="12"/>
     </row>
     <row r="12" spans="3:28" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="28"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="48"/>
       <c r="R12" s="12"/>
       <c r="S12" s="12"/>
       <c r="T12" s="12"/>
@@ -1273,31 +1406,31 @@
       <c r="AB12" s="12"/>
     </row>
     <row r="13" spans="3:28" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="38" t="s">
+      <c r="D13" s="51"/>
+      <c r="E13" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="39" t="s">
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="35" t="s">
+      <c r="I13" s="54"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="N13" s="35"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="43" t="s">
+      <c r="N13" s="53"/>
+      <c r="O13" s="53"/>
+      <c r="P13" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="Q13" s="43"/>
+      <c r="Q13" s="49"/>
       <c r="R13" s="16"/>
       <c r="S13" s="16"/>
       <c r="T13" s="16"/>
@@ -1425,21 +1558,21 @@
       <c r="AB16" s="12"/>
     </row>
     <row r="17" spans="3:28" x14ac:dyDescent="0.25">
-      <c r="C17" s="47"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="41"/>
-      <c r="N17" s="41"/>
-      <c r="O17" s="41"/>
-      <c r="P17" s="41"/>
-      <c r="Q17" s="41"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="28"/>
       <c r="R17" s="12"/>
       <c r="S17" s="12"/>
       <c r="T17" s="12"/>
@@ -1453,27 +1586,27 @@
       <c r="AB17" s="12"/>
     </row>
     <row r="18" spans="3:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="28"/>
-      <c r="S18" s="28"/>
-      <c r="T18" s="28"/>
-      <c r="U18" s="28"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="48"/>
+      <c r="O18" s="48"/>
+      <c r="P18" s="48"/>
+      <c r="Q18" s="48"/>
+      <c r="R18" s="48"/>
+      <c r="S18" s="48"/>
+      <c r="T18" s="48"/>
+      <c r="U18" s="48"/>
       <c r="V18" s="12"/>
       <c r="W18" s="12"/>
       <c r="X18" s="12"/>
@@ -1483,35 +1616,35 @@
       <c r="AB18" s="12"/>
     </row>
     <row r="19" spans="3:28" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="38" t="s">
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="39" t="s">
+      <c r="G19" s="52"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="39"/>
-      <c r="N19" s="39"/>
-      <c r="O19" s="35" t="s">
+      <c r="J19" s="54"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="54"/>
+      <c r="N19" s="54"/>
+      <c r="O19" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="35"/>
-      <c r="R19" s="35"/>
-      <c r="S19" s="43" t="s">
+      <c r="P19" s="53"/>
+      <c r="Q19" s="53"/>
+      <c r="R19" s="53"/>
+      <c r="S19" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="T19" s="43"/>
-      <c r="U19" s="43"/>
+      <c r="T19" s="49"/>
+      <c r="U19" s="49"/>
       <c r="V19" s="16"/>
       <c r="W19" s="16"/>
       <c r="X19" s="16"/>
@@ -1642,12 +1775,12 @@
       <c r="AA22" s="13"/>
       <c r="AB22" s="12"/>
     </row>
-    <row r="23" spans="3:28" x14ac:dyDescent="0.25">
-      <c r="C23" s="54"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
+    <row r="23" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="34"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
@@ -1670,72 +1803,72 @@
       <c r="AA23" s="13"/>
       <c r="AB23" s="12"/>
     </row>
-    <row r="24" spans="3:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="28" t="s">
+    <row r="24" spans="3:28" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
-      <c r="O24" s="28"/>
-      <c r="P24" s="28"/>
-      <c r="Q24" s="28"/>
-      <c r="R24" s="28"/>
-      <c r="S24" s="28"/>
-      <c r="T24" s="28"/>
-      <c r="U24" s="28"/>
-      <c r="V24" s="28"/>
-      <c r="W24" s="28"/>
-      <c r="X24" s="28"/>
-      <c r="Y24" s="28"/>
-      <c r="Z24" s="28"/>
-      <c r="AA24" s="13"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="61"/>
+      <c r="K24" s="61"/>
+      <c r="L24" s="61"/>
+      <c r="M24" s="61"/>
+      <c r="N24" s="61"/>
+      <c r="O24" s="61"/>
+      <c r="P24" s="61"/>
+      <c r="Q24" s="61"/>
+      <c r="R24" s="61"/>
+      <c r="S24" s="61"/>
+      <c r="T24" s="61"/>
+      <c r="U24" s="61"/>
+      <c r="V24" s="61"/>
+      <c r="W24" s="61"/>
+      <c r="X24" s="61"/>
+      <c r="Y24" s="61"/>
+      <c r="Z24" s="61"/>
+      <c r="AA24" s="62"/>
       <c r="AB24" s="12"/>
     </row>
     <row r="25" spans="3:28" x14ac:dyDescent="0.25">
-      <c r="C25" s="36" t="s">
+      <c r="C25" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="38" t="s">
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="35" t="s">
+      <c r="G25" s="57"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="57"/>
+      <c r="K25" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="35"/>
-      <c r="O25" s="39" t="s">
+      <c r="L25" s="58"/>
+      <c r="M25" s="58"/>
+      <c r="N25" s="58"/>
+      <c r="O25" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="P25" s="39"/>
-      <c r="Q25" s="39"/>
-      <c r="R25" s="39"/>
-      <c r="S25" s="39"/>
-      <c r="T25" s="39"/>
-      <c r="U25" s="39"/>
-      <c r="V25" s="39"/>
-      <c r="W25" s="39"/>
-      <c r="X25" s="43" t="s">
+      <c r="P25" s="59"/>
+      <c r="Q25" s="59"/>
+      <c r="R25" s="59"/>
+      <c r="S25" s="59"/>
+      <c r="T25" s="59"/>
+      <c r="U25" s="59"/>
+      <c r="V25" s="59"/>
+      <c r="W25" s="59"/>
+      <c r="X25" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="Y25" s="43"/>
-      <c r="Z25" s="43"/>
-      <c r="AA25" s="13"/>
+      <c r="Y25" s="64"/>
+      <c r="Z25" s="64"/>
+      <c r="AA25" s="65"/>
       <c r="AB25" s="12"/>
     </row>
     <row r="26" spans="3:28" x14ac:dyDescent="0.25">
@@ -1799,7 +1932,7 @@
       <c r="V26" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="W26" s="45" t="s">
+      <c r="W26" s="31" t="s">
         <v>2</v>
       </c>
       <c r="X26" s="6" t="s">
@@ -1811,7 +1944,9 @@
       <c r="Z26" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AA26" s="13"/>
+      <c r="AA26" s="31" t="s">
+        <v>2</v>
+      </c>
       <c r="AB26" s="12"/>
     </row>
     <row r="27" spans="3:28" x14ac:dyDescent="0.25">
@@ -1839,7 +1974,7 @@
       <c r="X27" s="1"/>
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
-      <c r="AA27" s="13"/>
+      <c r="AA27" s="10"/>
       <c r="AB27" s="12"/>
     </row>
     <row r="28" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1867,15 +2002,15 @@
       <c r="X28" s="22"/>
       <c r="Y28" s="22"/>
       <c r="Z28" s="22"/>
-      <c r="AA28" s="26"/>
+      <c r="AA28" s="23"/>
       <c r="AB28" s="12"/>
     </row>
     <row r="29" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C29" s="12"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
@@ -1889,9 +2024,9 @@
       <c r="R29" s="12"/>
       <c r="S29" s="12"/>
       <c r="T29" s="12"/>
-      <c r="U29" s="46"/>
-      <c r="V29" s="46"/>
-      <c r="W29" s="46"/>
+      <c r="U29" s="32"/>
+      <c r="V29" s="32"/>
+      <c r="W29" s="32"/>
       <c r="X29" s="12"/>
       <c r="Y29" s="12"/>
       <c r="Z29" s="12"/>
@@ -1925,141 +2060,141 @@
       <c r="AA30" s="12"/>
     </row>
     <row r="31" spans="3:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="48" t="s">
+      <c r="C31" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="49"/>
-      <c r="I31" s="49"/>
-      <c r="J31" s="49"/>
-      <c r="K31" s="49"/>
-      <c r="L31" s="49"/>
-      <c r="M31" s="49"/>
-      <c r="N31" s="49"/>
-      <c r="O31" s="49"/>
-      <c r="P31" s="49"/>
-      <c r="Q31" s="49"/>
-      <c r="R31" s="49"/>
-      <c r="S31" s="49"/>
-      <c r="T31" s="49"/>
-      <c r="U31" s="49"/>
-      <c r="V31" s="49"/>
-      <c r="W31" s="49"/>
-      <c r="X31" s="49"/>
-      <c r="Y31" s="49"/>
-      <c r="Z31" s="49"/>
-      <c r="AA31" s="50"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="42"/>
+      <c r="M31" s="42"/>
+      <c r="N31" s="42"/>
+      <c r="O31" s="42"/>
+      <c r="P31" s="42"/>
+      <c r="Q31" s="42"/>
+      <c r="R31" s="42"/>
+      <c r="S31" s="42"/>
+      <c r="T31" s="42"/>
+      <c r="U31" s="42"/>
+      <c r="V31" s="42"/>
+      <c r="W31" s="42"/>
+      <c r="X31" s="42"/>
+      <c r="Y31" s="42"/>
+      <c r="Z31" s="42"/>
+      <c r="AA31" s="43"/>
     </row>
     <row r="32" spans="3:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="51"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="52"/>
-      <c r="J32" s="52"/>
-      <c r="K32" s="52"/>
-      <c r="L32" s="52"/>
-      <c r="M32" s="52"/>
-      <c r="N32" s="52"/>
-      <c r="O32" s="52"/>
-      <c r="P32" s="52"/>
-      <c r="Q32" s="52"/>
-      <c r="R32" s="52"/>
-      <c r="S32" s="52"/>
-      <c r="T32" s="52"/>
-      <c r="U32" s="52"/>
-      <c r="V32" s="52"/>
-      <c r="W32" s="52"/>
-      <c r="X32" s="52"/>
-      <c r="Y32" s="52"/>
-      <c r="Z32" s="52"/>
-      <c r="AA32" s="53"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="45"/>
+      <c r="M32" s="45"/>
+      <c r="N32" s="45"/>
+      <c r="O32" s="45"/>
+      <c r="P32" s="45"/>
+      <c r="Q32" s="45"/>
+      <c r="R32" s="45"/>
+      <c r="S32" s="45"/>
+      <c r="T32" s="45"/>
+      <c r="U32" s="45"/>
+      <c r="V32" s="45"/>
+      <c r="W32" s="45"/>
+      <c r="X32" s="45"/>
+      <c r="Y32" s="45"/>
+      <c r="Z32" s="45"/>
+      <c r="AA32" s="46"/>
     </row>
     <row r="33" spans="3:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="51"/>
-      <c r="D33" s="52"/>
-      <c r="E33" s="52"/>
-      <c r="F33" s="52"/>
-      <c r="G33" s="52"/>
-      <c r="H33" s="52"/>
-      <c r="I33" s="52"/>
-      <c r="J33" s="52"/>
-      <c r="K33" s="52"/>
-      <c r="L33" s="52"/>
-      <c r="M33" s="52"/>
-      <c r="N33" s="52"/>
-      <c r="O33" s="52"/>
-      <c r="P33" s="52"/>
-      <c r="Q33" s="52"/>
-      <c r="R33" s="52"/>
-      <c r="S33" s="52"/>
-      <c r="T33" s="52"/>
-      <c r="U33" s="52"/>
-      <c r="V33" s="52"/>
-      <c r="W33" s="52"/>
-      <c r="X33" s="52"/>
-      <c r="Y33" s="52"/>
-      <c r="Z33" s="52"/>
-      <c r="AA33" s="53"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="45"/>
+      <c r="M33" s="45"/>
+      <c r="N33" s="45"/>
+      <c r="O33" s="45"/>
+      <c r="P33" s="45"/>
+      <c r="Q33" s="45"/>
+      <c r="R33" s="45"/>
+      <c r="S33" s="45"/>
+      <c r="T33" s="45"/>
+      <c r="U33" s="45"/>
+      <c r="V33" s="45"/>
+      <c r="W33" s="45"/>
+      <c r="X33" s="45"/>
+      <c r="Y33" s="45"/>
+      <c r="Z33" s="45"/>
+      <c r="AA33" s="46"/>
     </row>
     <row r="34" spans="3:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="51"/>
-      <c r="D34" s="52"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="52"/>
-      <c r="J34" s="52"/>
-      <c r="K34" s="52"/>
-      <c r="L34" s="52"/>
-      <c r="M34" s="52"/>
-      <c r="N34" s="52"/>
-      <c r="O34" s="52"/>
-      <c r="P34" s="52"/>
-      <c r="Q34" s="52"/>
-      <c r="R34" s="52"/>
-      <c r="S34" s="52"/>
-      <c r="T34" s="52"/>
-      <c r="U34" s="52"/>
-      <c r="V34" s="52"/>
-      <c r="W34" s="52"/>
-      <c r="X34" s="52"/>
-      <c r="Y34" s="52"/>
-      <c r="Z34" s="52"/>
-      <c r="AA34" s="53"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="45"/>
+      <c r="L34" s="45"/>
+      <c r="M34" s="45"/>
+      <c r="N34" s="45"/>
+      <c r="O34" s="45"/>
+      <c r="P34" s="45"/>
+      <c r="Q34" s="45"/>
+      <c r="R34" s="45"/>
+      <c r="S34" s="45"/>
+      <c r="T34" s="45"/>
+      <c r="U34" s="45"/>
+      <c r="V34" s="45"/>
+      <c r="W34" s="45"/>
+      <c r="X34" s="45"/>
+      <c r="Y34" s="45"/>
+      <c r="Z34" s="45"/>
+      <c r="AA34" s="46"/>
     </row>
     <row r="35" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C35" s="51"/>
-      <c r="D35" s="52"/>
-      <c r="E35" s="52"/>
-      <c r="F35" s="52"/>
-      <c r="G35" s="52"/>
-      <c r="H35" s="52"/>
-      <c r="I35" s="52"/>
-      <c r="J35" s="52"/>
-      <c r="K35" s="52"/>
-      <c r="L35" s="52"/>
-      <c r="M35" s="52"/>
-      <c r="N35" s="52"/>
-      <c r="O35" s="52"/>
-      <c r="P35" s="52"/>
-      <c r="Q35" s="52"/>
-      <c r="R35" s="52"/>
-      <c r="S35" s="52"/>
-      <c r="T35" s="52"/>
-      <c r="U35" s="52"/>
-      <c r="V35" s="52"/>
-      <c r="W35" s="52"/>
-      <c r="X35" s="52"/>
-      <c r="Y35" s="52"/>
-      <c r="Z35" s="52"/>
-      <c r="AA35" s="53"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="45"/>
+      <c r="K35" s="45"/>
+      <c r="L35" s="45"/>
+      <c r="M35" s="45"/>
+      <c r="N35" s="45"/>
+      <c r="O35" s="45"/>
+      <c r="P35" s="45"/>
+      <c r="Q35" s="45"/>
+      <c r="R35" s="45"/>
+      <c r="S35" s="45"/>
+      <c r="T35" s="45"/>
+      <c r="U35" s="45"/>
+      <c r="V35" s="45"/>
+      <c r="W35" s="45"/>
+      <c r="X35" s="45"/>
+      <c r="Y35" s="45"/>
+      <c r="Z35" s="45"/>
+      <c r="AA35" s="46"/>
     </row>
     <row r="36" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C36" s="11"/>
@@ -3515,12 +3650,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="X25:AA25"/>
+    <mergeCell ref="C24:AA24"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="I19:N19"/>
+    <mergeCell ref="C5:F5"/>
     <mergeCell ref="C1:AA3"/>
     <mergeCell ref="C31:AA35"/>
     <mergeCell ref="C18:U18"/>
     <mergeCell ref="S19:U19"/>
-    <mergeCell ref="X25:Z25"/>
-    <mergeCell ref="C24:Z24"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="C12:Q12"/>
@@ -3531,11 +3671,6 @@
     <mergeCell ref="K25:N25"/>
     <mergeCell ref="O25:W25"/>
     <mergeCell ref="H13:L13"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="I19:N19"/>
-    <mergeCell ref="C5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>